<commit_message>
Finalized Experiments with Participant Generation
</commit_message>
<xml_diff>
--- a/participants/participant_01/participant_01_task_orders.xlsx
+++ b/participants/participant_01/participant_01_task_orders.xlsx
@@ -7,11 +7,11 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="GNG_TO-16498730053485487" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="NB_TO-16498730087739527" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="RS_TO-16498730087739527" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="TOL_TO-16498730088359742" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="vSAT_TO-1649873008904751" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="GNG_TO-16502911110210803" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="NB_TO-16502911150057838" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="RS_TO-16502911150067856" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="TOL_TO-16502911150537822" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="vSAT_TO-16502911151178281" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -450,7 +450,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>go_stims-16498730053207505.csv</t>
+          <t>go_stims-16502911109880383.csv</t>
         </is>
       </c>
     </row>
@@ -460,7 +460,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>GNG_stims-16498730053318121.csv</t>
+          <t>GNG_stims-16502911110048633.csv</t>
         </is>
       </c>
     </row>
@@ -470,7 +470,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>go_stims-1649873005333781.csv</t>
+          <t>go_stims-16502911110058577.csv</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>GNG_stims-16498730053475857.csv</t>
+          <t>GNG_stims-16502911110200799.csv</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>TB-16498730078193333.csv</t>
+          <t>TB-16502911126407866.csv</t>
         </is>
       </c>
     </row>
@@ -526,7 +526,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>OB-16498730068512561.csv</t>
+          <t>OB-1650291112298637.csv</t>
         </is>
       </c>
     </row>
@@ -536,7 +536,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>OB-16498730062957468.csv</t>
+          <t>ZB-match_3-16502911117307928.csv</t>
         </is>
       </c>
     </row>
@@ -546,7 +546,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ZB-match_2-16498730055910485.csv</t>
+          <t>ZB-match_0-16502911111646838.csv</t>
         </is>
       </c>
     </row>
@@ -556,7 +556,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ZB-match_8-16498730059054494.csv</t>
+          <t>TB-16502911149827845.csv</t>
         </is>
       </c>
     </row>
@@ -566,7 +566,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>OB-1649873006113257.csv</t>
+          <t>TB-16502911147417824.csv</t>
         </is>
       </c>
     </row>
@@ -576,7 +576,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>TB-16498730070168839.csv</t>
+          <t>OB-16502911120066025.csv</t>
         </is>
       </c>
     </row>
@@ -586,7 +586,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>TB-16498730087586014.csv</t>
+          <t>ZB-match_9-16502911113343065.csv</t>
         </is>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ZB-match_4-1649873005823541.csv</t>
+          <t>OB-16502911123648126.csv</t>
         </is>
       </c>
     </row>
@@ -632,7 +632,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>eyes closed</t>
+          <t>eyes open</t>
         </is>
       </c>
     </row>
@@ -642,7 +642,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>eyes open</t>
+          <t>eyes closed</t>
         </is>
       </c>
     </row>
@@ -678,7 +678,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MM_stims-16498730087890532.csv</t>
+          <t>MM_stims-16502911150217834.csv</t>
         </is>
       </c>
     </row>
@@ -688,7 +688,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ZM_stims-16498730087759516.csv</t>
+          <t>ZM_stims-16502911150097883.csv</t>
         </is>
       </c>
     </row>
@@ -698,7 +698,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MM_stims-16498730088196554.csv</t>
+          <t>MM_stims-16502911150378237.csv</t>
         </is>
       </c>
     </row>
@@ -708,7 +708,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ZM_stims-1649873008790021.csv</t>
+          <t>ZM_stims-16502911150227823.csv</t>
         </is>
       </c>
     </row>
@@ -718,7 +718,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MM_stims-16498730088349738.csv</t>
+          <t>MM_stims-16502911150537822.csv</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ZM_stims-16498730088196554.csv</t>
+          <t>ZM_stims-1650291115038788.csv</t>
         </is>
       </c>
     </row>
@@ -764,7 +764,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SAT_stims-16498730088379748.csv</t>
+          <t>vSAT_stims-16502911150857868.csv</t>
         </is>
       </c>
     </row>
@@ -774,7 +774,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>vSAT_stims-164987300888831.csv</t>
+          <t>vSAT_stims-16502911151017828.csv</t>
         </is>
       </c>
     </row>
@@ -784,7 +784,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SAT_stims-16498730088575935.csv</t>
+          <t>SAT_stims-16502911150567834.csv</t>
         </is>
       </c>
     </row>
@@ -794,7 +794,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>vSAT_stims-16498730088728385.csv</t>
+          <t>SAT_stims-16502911150697823.csv</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed Stimulus Absolute Timestamps
</commit_message>
<xml_diff>
--- a/participants/participant_01/participant_01_task_orders.xlsx
+++ b/participants/participant_01/participant_01_task_orders.xlsx
@@ -7,11 +7,11 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="GNG_TO-16502911110210803" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="NB_TO-16502911150057838" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="RS_TO-16502911150067856" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="TOL_TO-16502911150537822" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="vSAT_TO-16502911151178281" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="GNG_TO-16504777688093762" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="NB_TO-16504777717933784" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="RS_TO-165047777179538" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="TOL_TO-16504777718573773" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="vSAT_TO-16504777719333835" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -450,7 +450,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>go_stims-16502911109880383.csv</t>
+          <t>go_stims-16504777687663777.csv</t>
         </is>
       </c>
     </row>
@@ -460,7 +460,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>GNG_stims-16502911110048633.csv</t>
+          <t>GNG_stims-165047776879141.csv</t>
         </is>
       </c>
     </row>
@@ -470,7 +470,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>go_stims-16502911110058577.csv</t>
+          <t>go_stims-1650477768794386.csv</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>GNG_stims-16502911110200799.csv</t>
+          <t>GNG_stims-16504777688083873.csv</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>TB-16502911126407866.csv</t>
+          <t>OB-165047777094038.csv</t>
         </is>
       </c>
     </row>
@@ -526,7 +526,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>OB-1650291112298637.csv</t>
+          <t>OB-16504777699983776.csv</t>
         </is>
       </c>
     </row>
@@ -536,7 +536,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ZB-match_3-16502911117307928.csv</t>
+          <t>TB-16504777716963847.csv</t>
         </is>
       </c>
     </row>
@@ -546,7 +546,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ZB-match_0-16502911111646838.csv</t>
+          <t>ZB-match_7-16504777697103772.csv</t>
         </is>
       </c>
     </row>
@@ -556,7 +556,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>TB-16502911149827845.csv</t>
+          <t>ZB-match_0-16504777692974021.csv</t>
         </is>
       </c>
     </row>
@@ -566,7 +566,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>TB-16502911147417824.csv</t>
+          <t>OB-16504777708383772.csv</t>
         </is>
       </c>
     </row>
@@ -576,7 +576,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>OB-16502911120066025.csv</t>
+          <t>TB-1650477771772381.csv</t>
         </is>
       </c>
     </row>
@@ -586,7 +586,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ZB-match_9-16502911113343065.csv</t>
+          <t>ZB-match_6-16504777693163767.csv</t>
         </is>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>OB-16502911123648126.csv</t>
+          <t>TB-1650477771444375.csv</t>
         </is>
       </c>
     </row>
@@ -632,7 +632,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>eyes open</t>
+          <t>eyes closed</t>
         </is>
       </c>
     </row>
@@ -642,7 +642,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>eyes closed</t>
+          <t>eyes open</t>
         </is>
       </c>
     </row>
@@ -678,7 +678,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MM_stims-16502911150217834.csv</t>
+          <t>MM_stims-16504777718093815.csv</t>
         </is>
       </c>
     </row>
@@ -688,7 +688,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ZM_stims-16502911150097883.csv</t>
+          <t>ZM_stims-16504777717973795.csv</t>
         </is>
       </c>
     </row>
@@ -698,7 +698,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MM_stims-16502911150378237.csv</t>
+          <t>MM_stims-16504777718403761.csv</t>
         </is>
       </c>
     </row>
@@ -708,7 +708,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ZM_stims-16502911150227823.csv</t>
+          <t>ZM_stims-16504777718103826.csv</t>
         </is>
       </c>
     </row>
@@ -718,7 +718,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MM_stims-16502911150537822.csv</t>
+          <t>MM_stims-16504777718573773.csv</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ZM_stims-1650291115038788.csv</t>
+          <t>ZM_stims-16504777718423893.csv</t>
         </is>
       </c>
     </row>
@@ -764,7 +764,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>vSAT_stims-16502911150857868.csv</t>
+          <t>SAT_stims-16504777718613951.csv</t>
         </is>
       </c>
     </row>
@@ -774,7 +774,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>vSAT_stims-16502911151017828.csv</t>
+          <t>vSAT_stims-16504777719014027.csv</t>
         </is>
       </c>
     </row>
@@ -784,7 +784,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SAT_stims-16502911150567834.csv</t>
+          <t>vSAT_stims-16504777719183755.csv</t>
         </is>
       </c>
     </row>
@@ -794,7 +794,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SAT_stims-16502911150697823.csv</t>
+          <t>SAT_stims-165047777188641.csv</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Practice tasks and final revisions
</commit_message>
<xml_diff>
--- a/participants/participant_01/participant_01_task_orders.xlsx
+++ b/participants/participant_01/participant_01_task_orders.xlsx
@@ -7,11 +7,11 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="GNG_TO-16504777688093762" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="NB_TO-16504777717933784" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="RS_TO-165047777179538" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="TOL_TO-16504777718573773" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="vSAT_TO-16504777719333835" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="GNG_TO-1650996061083159" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="NB_TO-1650996062440149" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="RS_TO-1650996062440149" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="TOL_TO-16509960624913397" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="vSAT_TO-16509960625793817" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -450,7 +450,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>go_stims-16504777687663777.csv</t>
+          <t>go_stims-16509960610509908.csv</t>
         </is>
       </c>
     </row>
@@ -460,7 +460,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>GNG_stims-165047776879141.csv</t>
+          <t>GNG_stims-1650996061067751.csv</t>
         </is>
       </c>
     </row>
@@ -470,7 +470,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>go_stims-1650477768794386.csv</t>
+          <t>go_stims-16509960610689428.csv</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>GNG_stims-16504777688083873.csv</t>
+          <t>GNG_stims-1650996061081884.csv</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>OB-165047777094038.csv</t>
+          <t>TB-1650996062146525.csv</t>
         </is>
       </c>
     </row>
@@ -526,7 +526,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>OB-16504777699983776.csv</t>
+          <t>ZB-match_8-16509960611798332.csv</t>
         </is>
       </c>
     </row>
@@ -536,7 +536,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>TB-16504777716963847.csv</t>
+          <t>TB-16509960624241474.csv</t>
         </is>
       </c>
     </row>
@@ -546,7 +546,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ZB-match_7-16504777697103772.csv</t>
+          <t>OB-16509960613337824.csv</t>
         </is>
       </c>
     </row>
@@ -556,7 +556,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ZB-match_0-16504777692974021.csv</t>
+          <t>ZB-match_9-16509960610898516.csv</t>
         </is>
       </c>
     </row>
@@ -566,7 +566,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>OB-16504777708383772.csv</t>
+          <t>ZB-match_3-16509960611267495.csv</t>
         </is>
       </c>
     </row>
@@ -576,7 +576,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>TB-1650477771772381.csv</t>
+          <t>TB-1650996061804661.csv</t>
         </is>
       </c>
     </row>
@@ -586,7 +586,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ZB-match_6-16504777693163767.csv</t>
+          <t>OB-16509960616194441.csv</t>
         </is>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>TB-1650477771444375.csv</t>
+          <t>OB-16509960617560792.csv</t>
         </is>
       </c>
     </row>
@@ -678,7 +678,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MM_stims-16504777718093815.csv</t>
+          <t>MM_stims-16509960624591658.csv</t>
         </is>
       </c>
     </row>
@@ -688,7 +688,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ZM_stims-16504777717973795.csv</t>
+          <t>ZM_stims-1650996062440149.csv</t>
         </is>
       </c>
     </row>
@@ -698,7 +698,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MM_stims-16504777718403761.csv</t>
+          <t>MM_stims-16509960624751606.csv</t>
         </is>
       </c>
     </row>
@@ -708,7 +708,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ZM_stims-16504777718103826.csv</t>
+          <t>ZM_stims-16509960624591658.csv</t>
         </is>
       </c>
     </row>
@@ -718,7 +718,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MM_stims-16504777718573773.csv</t>
+          <t>MM_stims-16509960624913397.csv</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ZM_stims-16504777718423893.csv</t>
+          <t>ZM_stims-16509960624751606.csv</t>
         </is>
       </c>
     </row>
@@ -764,7 +764,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SAT_stims-16504777718613951.csv</t>
+          <t>vSAT_stims-16509960625331023.csv</t>
         </is>
       </c>
     </row>
@@ -774,7 +774,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>vSAT_stims-16504777719014027.csv</t>
+          <t>vSAT_stims-16509960625633826.csv</t>
         </is>
       </c>
     </row>
@@ -784,7 +784,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>vSAT_stims-16504777719183755.csv</t>
+          <t>SAT_stims-1650996062492957.csv</t>
         </is>
       </c>
     </row>
@@ -794,7 +794,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SAT_stims-165047777188641.csv</t>
+          <t>SAT_stims-16509960625089948.csv</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Textbox response formatting fix
</commit_message>
<xml_diff>
--- a/participants/participant_01/participant_01_task_orders.xlsx
+++ b/participants/participant_01/participant_01_task_orders.xlsx
@@ -7,11 +7,11 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="GNG_TO-1650996061083159" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="NB_TO-1650996062440149" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="RS_TO-1650996062440149" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="TOL_TO-16509960624913397" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="vSAT_TO-16509960625793817" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="GNG_TO-16511686411348996" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="NB_TO-16511686461013448" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="RS_TO-16511686461023467" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="TOL_TO-16511686461653464" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="vSAT_TO-16511686462283473" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -450,7 +450,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>go_stims-16509960610509908.csv</t>
+          <t>go_stims-16511686411053183.csv</t>
         </is>
       </c>
     </row>
@@ -460,7 +460,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>GNG_stims-1650996061067751.csv</t>
+          <t>GNG_stims-16511686411181998.csv</t>
         </is>
       </c>
     </row>
@@ -470,7 +470,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>go_stims-16509960610689428.csv</t>
+          <t>go_stims-16511686411201637.csv</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>GNG_stims-1650996061081884.csv</t>
+          <t>GNG_stims-16511686411348996.csv</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>TB-1650996062146525.csv</t>
+          <t>ZB-match_8-16511686414114819.csv</t>
         </is>
       </c>
     </row>
@@ -526,7 +526,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ZB-match_8-16509960611798332.csv</t>
+          <t>TB-16511686433830547.csv</t>
         </is>
       </c>
     </row>
@@ -536,7 +536,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>TB-16509960624241474.csv</t>
+          <t>OB-1651168642279237.csv</t>
         </is>
       </c>
     </row>
@@ -546,7 +546,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>OB-16509960613337824.csv</t>
+          <t>TB-16511686460863428.csv</t>
         </is>
       </c>
     </row>
@@ -556,7 +556,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ZB-match_9-16509960610898516.csv</t>
+          <t>OB-1651168641982838.csv</t>
         </is>
       </c>
     </row>
@@ -566,7 +566,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ZB-match_3-16509960611267495.csv</t>
+          <t>ZB-match_7-1651168641581166.csv</t>
         </is>
       </c>
     </row>
@@ -576,7 +576,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>TB-1650996061804661.csv</t>
+          <t>OB-16511686417823737.csv</t>
         </is>
       </c>
     </row>
@@ -586,7 +586,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>OB-16509960616194441.csv</t>
+          <t>ZB-match_6-16511686412617369.csv</t>
         </is>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>OB-16509960617560792.csv</t>
+          <t>TB-16511686446970322.csv</t>
         </is>
       </c>
     </row>
@@ -632,7 +632,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>eyes closed</t>
+          <t>eyes open</t>
         </is>
       </c>
     </row>
@@ -642,7 +642,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>eyes open</t>
+          <t>eyes closed</t>
         </is>
       </c>
     </row>
@@ -678,7 +678,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MM_stims-16509960624591658.csv</t>
+          <t>MM_stims-16511686461173463.csv</t>
         </is>
       </c>
     </row>
@@ -688,7 +688,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ZM_stims-1650996062440149.csv</t>
+          <t>ZM_stims-1651168646104346.csv</t>
         </is>
       </c>
     </row>
@@ -698,7 +698,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MM_stims-16509960624751606.csv</t>
+          <t>MM_stims-16511686461483457.csv</t>
         </is>
       </c>
     </row>
@@ -708,7 +708,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ZM_stims-16509960624591658.csv</t>
+          <t>ZM_stims-16511686461183453.csv</t>
         </is>
       </c>
     </row>
@@ -718,7 +718,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MM_stims-16509960624913397.csv</t>
+          <t>MM_stims-16511686461643467.csv</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ZM_stims-16509960624751606.csv</t>
+          <t>ZM_stims-16511686461493454.csv</t>
         </is>
       </c>
     </row>
@@ -764,7 +764,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>vSAT_stims-16509960625331023.csv</t>
+          <t>SAT_stims-16511686461683457.csv</t>
         </is>
       </c>
     </row>
@@ -774,7 +774,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>vSAT_stims-16509960625633826.csv</t>
+          <t>vSAT_stims-16511686462133448.csv</t>
         </is>
       </c>
     </row>
@@ -784,7 +784,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SAT_stims-1650996062492957.csv</t>
+          <t>vSAT_stims-1651168646196379.csv</t>
         </is>
       </c>
     </row>
@@ -794,7 +794,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SAT_stims-16509960625089948.csv</t>
+          <t>SAT_stims-16511686461803775.csv</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Improved accuracy of stimulus presentation time-logging
</commit_message>
<xml_diff>
--- a/participants/participant_01/participant_01_task_orders.xlsx
+++ b/participants/participant_01/participant_01_task_orders.xlsx
@@ -7,11 +7,11 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="GNG_TO-16511686411348996" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="NB_TO-16511686461013448" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="RS_TO-16511686461023467" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="TOL_TO-16511686461653464" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="vSAT_TO-16511686462283473" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="GNG_TO-16512554784045432" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="NB_TO-16512554798627553" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="RS_TO-1651255479863755" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="TOL_TO-1651255479925753" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="vSAT_TO-16512554800197537" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -450,7 +450,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>go_stims-16511686411053183.csv</t>
+          <t>go_stims-1651255478362964.csv</t>
         </is>
       </c>
     </row>
@@ -460,7 +460,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>GNG_stims-16511686411181998.csv</t>
+          <t>GNG_stims-16512554783875763.csv</t>
         </is>
       </c>
     </row>
@@ -470,7 +470,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>go_stims-16511686411201637.csv</t>
+          <t>go_stims-16512554783895414.csv</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>GNG_stims-16511686411348996.csv</t>
+          <t>GNG_stims-16512554784035466.csv</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ZB-match_8-16511686414114819.csv</t>
+          <t>TB-16512554795927608.csv</t>
         </is>
       </c>
     </row>
@@ -526,7 +526,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>TB-16511686433830547.csv</t>
+          <t>ZB-match_1-1651255478739152.csv</t>
         </is>
       </c>
     </row>
@@ -536,7 +536,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>OB-1651168642279237.csv</t>
+          <t>OB-16512554794267561.csv</t>
         </is>
       </c>
     </row>
@@ -546,7 +546,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>TB-16511686460863428.csv</t>
+          <t>ZB-match_5-16512554786345272.csv</t>
         </is>
       </c>
     </row>
@@ -556,7 +556,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>OB-1651168641982838.csv</t>
+          <t>TB-16512554796827562.csv</t>
         </is>
       </c>
     </row>
@@ -566,7 +566,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ZB-match_7-1651168641581166.csv</t>
+          <t>OB-16512554790460126.csv</t>
         </is>
       </c>
     </row>
@@ -576,7 +576,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>OB-16511686417823737.csv</t>
+          <t>OB-16512554791851053.csv</t>
         </is>
       </c>
     </row>
@@ -586,7 +586,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ZB-match_6-16511686412617369.csv</t>
+          <t>ZB-match_8-16512554787128506.csv</t>
         </is>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>TB-16511686446970322.csv</t>
+          <t>TB-16512554798457994.csv</t>
         </is>
       </c>
     </row>
@@ -632,7 +632,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>eyes open</t>
+          <t>eyes closed</t>
         </is>
       </c>
     </row>
@@ -642,7 +642,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>eyes closed</t>
+          <t>eyes open</t>
         </is>
       </c>
     </row>
@@ -678,7 +678,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MM_stims-16511686461173463.csv</t>
+          <t>MM_stims-16512554798787553.csv</t>
         </is>
       </c>
     </row>
@@ -688,7 +688,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ZM_stims-1651168646104346.csv</t>
+          <t>ZM_stims-16512554798657575.csv</t>
         </is>
       </c>
     </row>
@@ -698,7 +698,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MM_stims-16511686461483457.csv</t>
+          <t>MM_stims-1651255479909795.csv</t>
         </is>
       </c>
     </row>
@@ -708,7 +708,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ZM_stims-16511686461183453.csv</t>
+          <t>ZM_stims-1651255479879758.csv</t>
         </is>
       </c>
     </row>
@@ -718,7 +718,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MM_stims-16511686461643467.csv</t>
+          <t>MM_stims-1651255479925753.csv</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ZM_stims-16511686461493454.csv</t>
+          <t>ZM_stims-16512554799107559.csv</t>
         </is>
       </c>
     </row>
@@ -764,7 +764,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SAT_stims-16511686461683457.csv</t>
+          <t>vSAT_stims-1651255479972755.csv</t>
         </is>
       </c>
     </row>
@@ -774,7 +774,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>vSAT_stims-16511686462133448.csv</t>
+          <t>SAT_stims-16512554799577544.csv</t>
         </is>
       </c>
     </row>
@@ -784,7 +784,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>vSAT_stims-1651168646196379.csv</t>
+          <t>vSAT_stims-1651255480003753.csv</t>
         </is>
       </c>
     </row>
@@ -794,7 +794,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SAT_stims-16511686461803775.csv</t>
+          <t>SAT_stims-16512554799307566.csv</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Created experiment order generation script
</commit_message>
<xml_diff>
--- a/participants/participant_01/participant_01_task_orders.xlsx
+++ b/participants/participant_01/participant_01_task_orders.xlsx
@@ -7,11 +7,11 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="GNG_TO-16512554784045432" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="NB_TO-16512554798627553" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="RS_TO-1651255479863755" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="TOL_TO-1651255479925753" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="vSAT_TO-16512554800197537" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="vSAT_TO-16515889079379363" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="NB_TO-16515889100982873" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="TOL_TO-16515889101628957" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="GNG_TO-16515889101945648" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="RS_TO-1651588910196574" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -450,7 +450,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>go_stims-1651255478362964.csv</t>
+          <t>vSAT_stims-16515889079229376.csv</t>
         </is>
       </c>
     </row>
@@ -460,7 +460,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>GNG_stims-16512554783875763.csv</t>
+          <t>vSAT_stims-16515889079095068.csv</t>
         </is>
       </c>
     </row>
@@ -470,7 +470,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>go_stims-16512554783895414.csv</t>
+          <t>SAT_stims-16515889078813736.csv</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>GNG_stims-16512554784035466.csv</t>
+          <t>SAT_stims-16515889078942704.csv</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>TB-16512554795927608.csv</t>
+          <t>TB-16515889093069654.csv</t>
         </is>
       </c>
     </row>
@@ -526,7 +526,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ZB-match_1-1651255478739152.csv</t>
+          <t>OB-16515889091540277.csv</t>
         </is>
       </c>
     </row>
@@ -536,7 +536,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>OB-16512554794267561.csv</t>
+          <t>ZB-match_9-1651588908146809.csv</t>
         </is>
       </c>
     </row>
@@ -546,7 +546,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ZB-match_5-16512554786345272.csv</t>
+          <t>TB-16515889097006068.csv</t>
         </is>
       </c>
     </row>
@@ -556,7 +556,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>TB-16512554796827562.csv</t>
+          <t>TB-16515889100833914.csv</t>
         </is>
       </c>
     </row>
@@ -566,7 +566,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>OB-16512554790460126.csv</t>
+          <t>ZB-match_8-1651588908117809.csv</t>
         </is>
       </c>
     </row>
@@ -576,7 +576,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>OB-16512554791851053.csv</t>
+          <t>OB-16515889083232734.csv</t>
         </is>
       </c>
     </row>
@@ -586,7 +586,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ZB-match_8-16512554787128506.csv</t>
+          <t>OB-16515889088098276.csv</t>
         </is>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>TB-16512554798457994.csv</t>
+          <t>ZB-match_3-16515889082171187.csv</t>
         </is>
       </c>
     </row>
@@ -606,6 +606,158 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>task_order</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>MM_stims-16515889101141453.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ZM_stims-16515889101002276.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MM_stims-16515889101458697.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ZM_stims-16515889101151116.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>MM_stims-16515889101618998.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ZM_stims-16515889101468775.csv</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>task_order</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>go_stims-16515889101666865.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>GNG_stims-16515889101777232.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>go_stims-16515889101787825.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>GNG_stims-1651588910193426.csv</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -649,156 +801,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>task_order</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>MM_stims-16512554798787553.csv</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ZM_stims-16512554798657575.csv</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>MM_stims-1651255479909795.csv</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>ZM_stims-1651255479879758.csv</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>MM_stims-1651255479925753.csv</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>ZM_stims-16512554799107559.csv</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>task_order</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>vSAT_stims-1651255479972755.csv</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>SAT_stims-16512554799577544.csv</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>vSAT_stims-1651255480003753.csv</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>SAT_stims-16512554799307566.csv</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>